<commit_message>
add download pdf for preview
</commit_message>
<xml_diff>
--- a/response_output.xlsx
+++ b/response_output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3206,7 +3206,7 @@
   <pageMargins left="0.3937" right="0.3937" top="0.9843" bottom="0.3937" header="0.5118" footer="0.3937"/>
   <pageSetup orientation="portrait" paperSize="9" fitToHeight="0" fitToWidth="1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"微軟正黑體,粗體"&amp;20 2025/05/02&amp;C&amp;"微軟正黑體,粗體"&amp;20 黑貓宅配(第一批)&amp;R&amp;"微軟正黑體,粗體"&amp;20 第 &amp;P 頁，共 &amp;N 頁</oddHeader>
+    <oddHeader>&amp;L&amp;"微軟正黑體,粗體"&amp;20 2025/05/03&amp;C&amp;"微軟正黑體,粗體"&amp;20 黑貓宅配(第一批)&amp;R&amp;"微軟正黑體,粗體"&amp;20 第 &amp;P 頁，共 &amp;N 頁</oddHeader>
     <oddFooter/>
     <evenHeader/>
     <evenFooter/>

</xml_diff>